<commit_message>
fixing minor logging issues
</commit_message>
<xml_diff>
--- a/Otomatika.xlsx
+++ b/Otomatika.xlsx
@@ -476,21 +476,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>With Bowman’s loss to Latimer, the NY Democratic establishment strikes back</t>
+          <t>New rules are coming for PFAS in drinking water. See how your water tests.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Westchester’s George Latimer secured a quick and decisive win over Rep. Jamaal Bowman Tuesday night. Here’s what the outcome tells us.</t>
+          <t>A Gothamist analysis shows that the drinking water of 4.3 million New York and New Jersey residents has tested positive for so-called “forever chemicals.” See if you’re one of them.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -499,17 +499,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bowman loses to Latimer in NY Democratic primary shaped by Israel-Hamas war</t>
+          <t>With Bowman’s loss to Latimer, the NY Democratic establishment strikes back</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The 16th Congressional District that spans from northern Bronx to Westchester now ranks as the most expensive House primary in American history.</t>
+          <t>Westchester’s George Latimer secured a quick and decisive win over Rep. Jamaal Bowman Tuesday night. Here’s what the outcome tells us.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -522,17 +522,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Admission for Black students at NYC’s specialized high schools ticks up slightly, but remains low</t>
+          <t>Bowman loses to Latimer in NY Democratic primary shaped by Israel-Hamas war</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Instead of pushing for systemwide change, this administration applauds a mere 1% increase in offers to Black and Latinx students,” one advocate says.</t>
+          <t>The 16th Congressional District that spans from northern Bronx to Westchester now ranks as the most expensive House primary in American history.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -545,17 +545,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NYPD inspector accused of sloppy coverup of DUI crash after boozy night at Midtown bar</t>
+          <t>Admission for Black students at NYC’s specialized high schools ticks up slightly, but remains low</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Prosecutors said Deputy Inspector Paul Zangrilli scrambled to destroy evidence after he let his drunk girlfriend drive his unmarked police car.</t>
+          <t>“Instead of pushing for systemwide change, this administration applauds a mere 1% increase in offers to Black and Latinx students,” one advocate says.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -568,63 +568,63 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NYCHA’s not just a landlord. It's going to train young adults to work in construction.</t>
+          <t>NYPD inspector accused of sloppy coverup of DUI crash after boozy night at Midtown bar</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The $1.3 million grant from the U.S. Labor Department will fund the workforce development program for 40 months.</t>
+          <t>Prosecutors said Deputy Inspector Paul Zangrilli scrambled to destroy evidence after he let his drunk girlfriend drive his unmarked police car.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>James Beard Foundation announces Best Chef in New York</t>
+          <t>NYCHA’s not just a landlord. It's going to train young adults to work in construction.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>New York was iced out of many major categories this year.</t>
+          <t>The $1.3 million grant from the U.S. Labor Department will fund the workforce development program for 40 months.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NYC public schools will educate students and their families about safe gun storage</t>
+          <t>James Beard Foundation announces Best Chef in New York</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The announcement comes after a 14-year-old was accidentally shot and killed by his cousin, who was playing with a gun.</t>
+          <t>New York was iced out of many major categories this year.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -637,17 +637,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>How to start running in NYC: Fun routes, safety tips and where to get proper shoes</t>
+          <t>NYC public schools will educate students and their families about safe gun storage</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Go extremely slow, try to find a car-free area — even if it’s just a little park to run laps around — and don’t be afraid to dress like a highlighter.</t>
+          <t>The announcement comes after a 14-year-old was accidentally shot and killed by his cousin, who was playing with a gun.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -660,21 +660,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Early Addition: A lot of NYPD officers allegedly cheated on the sergeant's exam</t>
+          <t>How to start running in NYC: Fun routes, safety tips and where to get proper shoes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Because many of them still managed to fail the test, here are your early links: Fat Joe lobbying for hospital price transparency, Derek Jeter sold his castle, mixing chip flavors in one bag is a bad idea and more.</t>
+          <t>Go extremely slow, try to find a car-free area — even if it’s just a little park to run laps around — and don’t be afraid to dress like a highlighter.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://api-prod.gothamist.com/images/345866/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
+          <t>https://api-prod.gothamist.com/images/345911/fill-318x212%7Cformat-webp%7Cwebpquality-80/</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>

</xml_diff>